<commit_message>
Total descuentos del 30112024
agregue los descuentos por vales y por color
</commit_message>
<xml_diff>
--- a/2. Descuentos/2. NOV_16_25.xlsx
+++ b/2. Descuentos/2. NOV_16_25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\AA GiHub\ForeverChic\2. Descuentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16308EF3-7C6A-47A7-8F5F-71431D0B50C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D78CBE-7DE2-4E2C-B940-3766C54F6FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{66B822A5-C23A-4837-8B6D-D5DF52A9F78C}"/>
   </bookViews>
@@ -745,7 +745,7 @@
   <dimension ref="A1:F200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.25" x14ac:dyDescent="0.25"/>
@@ -792,7 +792,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="4">
-        <v>1</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -814,7 +814,7 @@
       </c>
       <c r="E3" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -835,7 +835,7 @@
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>